<commit_message>
Completed four exercises for week 1
</commit_message>
<xml_diff>
--- a/notebooks/class_5/week_1/data/original/employment-statistics-by-industry.xlsx
+++ b/notebooks/class_5/week_1/data/original/employment-statistics-by-industry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/Library/CloudStorage/Dropbox/Code/practicaldatascience_book/notebooks/class_5/week_1/data/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2F01AD2-A5B9-724E-BB94-1CFD10E71D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48725981-94DB-2248-93AC-1021DBCB1C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36060" yWindow="-2080" windowWidth="28040" windowHeight="16940" activeTab="2" xr2:uid="{2DCD5C83-11D7-144A-A3F6-92F73E5CBEE5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{2DCD5C83-11D7-144A-A3F6-92F73E5CBEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -4470,7 +4470,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4547,7 +4547,7 @@
         <v>143393</v>
       </c>
       <c r="K2" s="1">
-        <f>J2/$J$2*100</f>
+        <f t="shared" ref="K2:K23" si="0">J2/$J$2*100</f>
         <v>100</v>
       </c>
     </row>
@@ -4583,7 +4583,7 @@
         <v>18904</v>
       </c>
       <c r="K3" s="1">
-        <f>J3/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>13.18334925693723</v>
       </c>
       <c r="L3" s="1">
@@ -4623,7 +4623,7 @@
         <v>16153</v>
       </c>
       <c r="K4" s="1">
-        <f>J4/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>11.264845564288354</v>
       </c>
       <c r="L4" s="1">
@@ -4663,7 +4663,7 @@
         <v>13704</v>
       </c>
       <c r="K5" s="1">
-        <f>J5/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>9.5569518735224186</v>
       </c>
       <c r="L5" s="1">
@@ -4703,7 +4703,7 @@
         <v>12523</v>
       </c>
       <c r="K6" s="1">
-        <f>J6/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>8.733341237019939</v>
       </c>
       <c r="L6" s="1">
@@ -4743,7 +4743,7 @@
         <v>10962</v>
       </c>
       <c r="K7" s="1">
-        <f>J7/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>7.6447246378833</v>
       </c>
       <c r="L7" s="1">
@@ -4783,7 +4783,7 @@
         <v>10216</v>
       </c>
       <c r="K8" s="1">
-        <f>J8/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>7.1244760901857136</v>
       </c>
       <c r="L8" s="1">
@@ -4823,7 +4823,7 @@
         <v>8917</v>
       </c>
       <c r="K9" s="1">
-        <f>J9/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>6.2185741284442058</v>
       </c>
       <c r="L9" s="1">
@@ -4863,7 +4863,7 @@
         <v>7699</v>
       </c>
       <c r="K10" s="1">
-        <f>J10/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>5.3691602797905063</v>
       </c>
       <c r="L10" s="1">
@@ -4903,7 +4903,7 @@
         <v>6570</v>
       </c>
       <c r="K11" s="1">
-        <f>J11/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.5818136171221751</v>
       </c>
       <c r="L11" s="1">
@@ -4943,7 +4943,7 @@
         <v>6232</v>
       </c>
       <c r="K12" s="1">
-        <f>J12/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.346097787200212</v>
       </c>
       <c r="L12" s="1">
@@ -4983,7 +4983,7 @@
         <v>6085</v>
       </c>
       <c r="K13" s="1">
-        <f>J13/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.2435823227075238</v>
       </c>
       <c r="L13" s="1">
@@ -5023,7 +5023,7 @@
         <v>5814</v>
       </c>
       <c r="K14" s="1">
-        <f>J14/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.0545912283026366</v>
       </c>
       <c r="L14" s="1">
@@ -5063,7 +5063,7 @@
         <v>4349</v>
       </c>
       <c r="K15" s="1">
-        <f>J15/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>3.032923503936733</v>
       </c>
       <c r="L15" s="1">
@@ -5103,7 +5103,7 @@
         <v>3465</v>
       </c>
       <c r="K16" s="1">
-        <f>J16/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>2.4164359487562153</v>
       </c>
       <c r="L16" s="1">
@@ -5143,7 +5143,7 @@
         <v>2870</v>
       </c>
       <c r="K17" s="1">
-        <f>J17/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>2.0014924020000975</v>
       </c>
       <c r="L17" s="1">
@@ -5183,7 +5183,7 @@
         <v>2476</v>
       </c>
       <c r="K18" s="1">
-        <f>J18/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>1.7267230617952063</v>
       </c>
       <c r="L18" s="1">
@@ -5223,7 +5223,7 @@
         <v>2249</v>
       </c>
       <c r="K19" s="1">
-        <f>J19/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>1.5684168683269057</v>
       </c>
       <c r="L19" s="1">
@@ -5263,7 +5263,7 @@
         <v>1888</v>
       </c>
       <c r="K20" s="1">
-        <f>J20/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>1.3166612038244545</v>
       </c>
       <c r="L20" s="1">
@@ -5303,7 +5303,7 @@
         <v>1219</v>
       </c>
       <c r="K21" s="1">
-        <f>J21/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>0.85011123276589518</v>
       </c>
       <c r="L21" s="1">
@@ -5343,7 +5343,7 @@
         <v>549</v>
       </c>
       <c r="K22" s="1">
-        <f>J22/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>0.38286387759514062</v>
       </c>
       <c r="L22" s="1">
@@ -5383,7 +5383,7 @@
         <v>548</v>
       </c>
       <c r="K23" s="1">
-        <f>J23/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>0.38216649348294546</v>
       </c>
       <c r="L23" s="1">
@@ -5406,13 +5406,13 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5483,7 +5483,7 @@
         <v>143393</v>
       </c>
       <c r="K2" s="1">
-        <f>J2/$J$2*100</f>
+        <f t="shared" ref="K2:K23" si="0">J2/$J$2*100</f>
         <v>100</v>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
         <v>18904</v>
       </c>
       <c r="K3" s="1">
-        <f>J3/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>13.18334925693723</v>
       </c>
       <c r="L3" s="1">
@@ -5559,7 +5559,7 @@
         <v>16153</v>
       </c>
       <c r="K4" s="1">
-        <f>J4/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>11.264845564288354</v>
       </c>
       <c r="L4" s="1">
@@ -5599,7 +5599,7 @@
         <v>13704</v>
       </c>
       <c r="K5" s="1">
-        <f>J5/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>9.5569518735224186</v>
       </c>
       <c r="L5" s="1">
@@ -5639,7 +5639,7 @@
         <v>12523</v>
       </c>
       <c r="K6" s="1">
-        <f>J6/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>8.733341237019939</v>
       </c>
       <c r="L6" s="1">
@@ -5679,7 +5679,7 @@
         <v>10962</v>
       </c>
       <c r="K7" s="1">
-        <f>J7/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>7.6447246378833</v>
       </c>
       <c r="L7" s="1">
@@ -5719,7 +5719,7 @@
         <v>10216</v>
       </c>
       <c r="K8" s="1">
-        <f>J8/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>7.1244760901857136</v>
       </c>
       <c r="L8" s="1">
@@ -5759,7 +5759,7 @@
         <v>8917</v>
       </c>
       <c r="K9" s="1">
-        <f>J9/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>6.2185741284442058</v>
       </c>
       <c r="L9" s="1">
@@ -5799,7 +5799,7 @@
         <v>7699</v>
       </c>
       <c r="K10" s="1">
-        <f>J10/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>5.3691602797905063</v>
       </c>
       <c r="L10" s="1">
@@ -5839,7 +5839,7 @@
         <v>6570</v>
       </c>
       <c r="K11" s="1">
-        <f>J11/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.5818136171221751</v>
       </c>
       <c r="L11" s="1">
@@ -5879,7 +5879,7 @@
         <v>6232</v>
       </c>
       <c r="K12" s="1">
-        <f>J12/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.346097787200212</v>
       </c>
       <c r="L12" s="1">
@@ -5919,7 +5919,7 @@
         <v>6085</v>
       </c>
       <c r="K13" s="1">
-        <f>J13/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.2435823227075238</v>
       </c>
       <c r="L13" s="1">
@@ -5959,7 +5959,7 @@
         <v>5814</v>
       </c>
       <c r="K14" s="1">
-        <f>J14/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>4.0545912283026366</v>
       </c>
       <c r="L14" s="1">
@@ -5999,7 +5999,7 @@
         <v>4349</v>
       </c>
       <c r="K15" s="1">
-        <f>J15/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>3.032923503936733</v>
       </c>
       <c r="L15" s="1">
@@ -6039,7 +6039,7 @@
         <v>3465</v>
       </c>
       <c r="K16" s="1">
-        <f>J16/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>2.4164359487562153</v>
       </c>
       <c r="L16" s="1">
@@ -6079,7 +6079,7 @@
         <v>2870</v>
       </c>
       <c r="K17" s="1">
-        <f>J17/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>2.0014924020000975</v>
       </c>
       <c r="L17" s="1">
@@ -6119,7 +6119,7 @@
         <v>2476</v>
       </c>
       <c r="K18" s="1">
-        <f>J18/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>1.7267230617952063</v>
       </c>
       <c r="L18" s="1">
@@ -6159,7 +6159,7 @@
         <v>2249</v>
       </c>
       <c r="K19" s="1">
-        <f>J19/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>1.5684168683269057</v>
       </c>
       <c r="L19" s="1">
@@ -6199,7 +6199,7 @@
         <v>1888</v>
       </c>
       <c r="K20" s="1">
-        <f>J20/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>1.3166612038244545</v>
       </c>
       <c r="L20" s="1">
@@ -6239,7 +6239,7 @@
         <v>1219</v>
       </c>
       <c r="K21" s="1">
-        <f>J21/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>0.85011123276589518</v>
       </c>
       <c r="L21" s="1">
@@ -6279,7 +6279,7 @@
         <v>549</v>
       </c>
       <c r="K22" s="1">
-        <f>J22/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>0.38286387759514062</v>
       </c>
       <c r="L22" s="1">
@@ -6319,7 +6319,7 @@
         <v>548</v>
       </c>
       <c r="K23" s="1">
-        <f>J23/$J$2*100</f>
+        <f t="shared" si="0"/>
         <v>0.38216649348294546</v>
       </c>
       <c r="L23" s="1">

</xml_diff>